<commit_message>
Updated with missing OOI Bar Codes, Added PAR scaling value
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP05MOAS-GL374_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_CP05MOAS-GL374_00003.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="3615" windowWidth="23295" windowHeight="9540" tabRatio="377"/>
+    <workbookView xWindow="4155" yWindow="3615" windowWidth="23295" windowHeight="9540" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,12 +35,12 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$79</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$360</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>Ref Des</t>
   </si>
@@ -167,6 +172,9 @@
   </si>
   <si>
     <t>EB Line</t>
+  </si>
+  <si>
+    <t>OL000351</t>
   </si>
 </sst>
 </file>
@@ -570,6 +578,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -617,7 +628,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -652,7 +663,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -863,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1424,7 @@
         <v>38</v>
       </c>
       <c r="H16" s="30">
-        <v>9.9999999999999995E-7</v>
+        <v>1</v>
       </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -1447,7 +1458,9 @@
       <c r="D18" s="14">
         <v>3</v>
       </c>
-      <c r="E18" s="14"/>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
       <c r="F18" s="18">
         <v>374</v>
       </c>

</xml_diff>

<commit_message>
glider 374 recovered - date entered
Cal Sheet Update:  entered the recovery date of glider 374 : 2016-08-09
05:30 UTC
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP05MOAS-GL374_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_CP05MOAS-GL374_00003.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leila/Documents/OOI_assmgt/asset-management/deployment/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="4160" yWindow="3620" windowWidth="23300" windowHeight="9540" tabRatio="377"/>
   </bookViews>
@@ -30,8 +35,11 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$79</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$360</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -40,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>Ref Des</t>
   </si>
@@ -181,7 +189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -298,6 +306,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue ,Helvetica,Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -469,9 +482,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="15" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -496,6 +506,7 @@
     <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -878,10 +889,10 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
@@ -891,45 +902,45 @@
     <col min="12" max="12" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:14" ht="28" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="15">
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -939,28 +950,28 @@
       <c r="C2" s="9">
         <v>374</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="24">
         <v>3</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="30">
         <v>42519</v>
       </c>
       <c r="F2" s="10">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="26" t="s">
+      <c r="G2" s="32">
+        <v>42591</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="27">
+      <c r="J2" s="26">
         <v>200</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="24" t="s">
         <v>39</v>
       </c>
       <c r="L2" s="8" t="s">
@@ -975,7 +986,7 @@
         <v>-70.36666666666666</v>
       </c>
     </row>
-    <row r="18" spans="8:8">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H18" t="s">
         <v>40</v>
       </c>
@@ -983,11 +994,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -999,7 +1005,7 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
@@ -1009,11 +1015,11 @@
     <col min="7" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30">
+    <row r="1" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1022,7 +1028,7 @@
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1035,7 +1041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
@@ -1070,7 +1076,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
@@ -1105,7 +1111,7 @@
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1140,7 +1146,7 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -1175,7 +1181,7 @@
       <c r="P5" s="17"/>
       <c r="Q5" s="17"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="14"/>
@@ -1194,7 +1200,7 @@
       <c r="P6" s="17"/>
       <c r="Q6" s="17"/>
     </row>
-    <row r="7" spans="1:17" s="5" customFormat="1">
+    <row r="7" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
@@ -1224,7 +1230,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:17" s="5" customFormat="1">
+    <row r="8" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
@@ -1254,7 +1260,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:17" s="5" customFormat="1">
+    <row r="9" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
@@ -1284,7 +1290,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:17" s="5" customFormat="1">
+    <row r="10" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
@@ -1314,7 +1320,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:17" s="5" customFormat="1">
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="14"/>
@@ -1328,7 +1334,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="5" customFormat="1">
+    <row r="12" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
@@ -1354,7 +1360,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="5" customFormat="1">
+    <row r="13" spans="1:17" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="14"/>
@@ -1368,7 +1374,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:17" s="5" customFormat="1">
+    <row r="14" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>26</v>
       </c>
@@ -1394,7 +1400,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:17" s="5" customFormat="1">
+    <row r="15" spans="1:17" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="14"/>
@@ -1408,7 +1414,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1">
+    <row r="16" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
@@ -1427,10 +1433,10 @@
       <c r="F16" s="18">
         <v>50157</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="31">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="I16" s="12"/>
@@ -1438,7 +1444,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" s="5" customFormat="1">
+    <row r="17" spans="1:12" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="14"/>
@@ -1452,7 +1458,7 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" s="5" customFormat="1">
+    <row r="18" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
@@ -1478,7 +1484,7 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" s="5" customFormat="1">
+    <row r="19" spans="1:12" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="14"/>
@@ -1495,10 +1501,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>